<commit_message>
Going back home to run 15 spheres 256 1024 mutex and finish the report
In other, completely unrelated news, Arsenal are about to get pumped daft at the Etihad
</commit_message>
<xml_diff>
--- a/CW1/Graphs/Graphs.xlsx
+++ b/CW1/Graphs/Graphs.xlsx
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="9">
   <si>
     <t>Parallel For</t>
   </si>
   <si>
     <t>Threads</t>
-  </si>
-  <si>
-    <t>4 samples</t>
   </si>
   <si>
     <t>Samples per Pixel</t>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>15 spheres</t>
+  </si>
+  <si>
+    <t>400x400</t>
+  </si>
+  <si>
+    <t>Home:</t>
   </si>
 </sst>
 </file>
@@ -432,6 +435,906 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>15 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>400 x 400</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$50:$M$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5009.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20233.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80070.399999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>328751.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B703-4282-A711-884D22CA7167}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$50:$N$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2013.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9010.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35544.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139375.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B703-4282-A711-884D22CA7167}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$50:$O$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9786.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37831.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150865.20000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B703-4282-A711-884D22CA7167}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>12 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$71:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACAC-404C-9D7A-C7B288F8DF0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$71:$J$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ACAC-404C-9D7A-C7B288F8DF0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$71:$K$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ACAC-404C-9D7A-C7B288F8DF0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>15 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$71:$N$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D988-4D63-BDDA-B06AF0D44524}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$71:$O$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D988-4D63-BDDA-B06AF0D44524}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$71:$P$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D988-4D63-BDDA-B06AF0D44524}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -970,6 +1873,1914 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3FD7-4005-9B94-586CB283C417}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Games Lab</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>9 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12560.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50097.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>198856.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>793702.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CD5-4635-96AA-EA77268F7153}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$27:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3652.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14532.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57514.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>229915.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6CD5-4635-96AA-EA77268F7153}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14769</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>236437</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6CD5-4635-96AA-EA77268F7153}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Games Lab</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>12 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$27:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12657.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50197.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200329.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>799601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A5C-40E0-AA96-233F7ED22E7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$27:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3557.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14356.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56290.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>224946.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2A5C-40E0-AA96-233F7ED22E7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$27:$J$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3696</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>231035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2A5C-40E0-AA96-233F7ED22E7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Games Lab</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>15 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$27:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16331.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64152.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>255877.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>999672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F311-4D89-91E6-34226ACF039C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$27:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4279.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17189.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67790.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>271312.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F311-4D89-91E6-34226ACF039C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$27:$O$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>275993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F311-4D89-91E6-34226ACF039C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>9 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>400 x 400</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3772.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15083.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60250.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242848.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4411-4C68-A7C2-2A64EA2AE011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$50:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1567.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8175.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32501.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125720.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4411-4C68-A7C2-2A64EA2AE011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$50:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8607.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34919.699999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>135913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4411-4C68-A7C2-2A64EA2AE011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>9 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>1024 x 1024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$71:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-230E-421D-9EA8-2B8A295308D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$71:$E$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-230E-421D-9EA8-2B8A295308D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$71:$F$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-230E-421D-9EA8-2B8A295308D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="39597184"/>
+        <c:axId val="39599488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39597184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (per pixel)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39599488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39597184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Home</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+              <a:t>12 Spheres</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1000"/>
+              <a:t>400 x 400</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$50:$H$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3849.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15581.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61686.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>255410.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6042-4FA0-9A12-58EE72AD66AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads w/Mutex</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]DefaultHomeVsGamesLab!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$50:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1570.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7754.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29593.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118001.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6042-4FA0-9A12-58EE72AD66AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Parallel For</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$50:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1669.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8350.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32279.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126670.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6042-4FA0-9A12-58EE72AD66AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1178,6 +3989,294 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1189,69 +4288,29 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="C3">
-            <v>27043</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>100863</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>427334</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>1709837</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>6587160</v>
-          </cell>
-        </row>
         <row r="12">
           <cell r="B12">
             <v>4</v>
-          </cell>
-          <cell r="C12">
-            <v>14611</v>
           </cell>
         </row>
         <row r="13">
           <cell r="B13">
             <v>16</v>
           </cell>
-          <cell r="C13">
-            <v>51657</v>
-          </cell>
         </row>
         <row r="14">
           <cell r="B14">
             <v>64</v>
-          </cell>
-          <cell r="C14">
-            <v>197122</v>
           </cell>
         </row>
         <row r="15">
           <cell r="B15">
             <v>256</v>
           </cell>
-          <cell r="C15">
-            <v>813115</v>
-          </cell>
         </row>
         <row r="16">
           <cell r="B16">
             <v>1024</v>
-          </cell>
-          <cell r="C16">
-            <v>3128357</v>
           </cell>
         </row>
       </sheetData>
@@ -1523,10 +4582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" activeCellId="2" sqref="C3 H3 M3"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="O95" sqref="O95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,24 +4596,24 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -1563,10 +4622,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
@@ -1575,10 +4634,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="N3" t="s">
         <v>1</v>
@@ -1739,37 +4798,698 @@
         <v>42047.8</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1024</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>12560.6</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3652.7</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3852</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27" s="1">
+        <v>12657.2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3557.4</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3696</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1">
+        <v>16331.7</v>
+      </c>
+      <c r="N27" s="1">
+        <v>4279.7</v>
+      </c>
+      <c r="O27" s="1">
+        <v>4353</v>
+      </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1">
+        <v>50097.4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>14532.8</v>
+      </c>
+      <c r="E28" s="1">
+        <v>14769</v>
+      </c>
+      <c r="G28">
+        <v>16</v>
+      </c>
+      <c r="H28" s="1">
+        <v>50197.7</v>
+      </c>
+      <c r="I28" s="1">
+        <v>14356.7</v>
+      </c>
+      <c r="J28" s="1">
+        <v>14317</v>
+      </c>
+      <c r="L28">
+        <v>16</v>
+      </c>
+      <c r="M28" s="1">
+        <v>64152.6</v>
+      </c>
+      <c r="N28" s="1">
+        <v>17189.7</v>
+      </c>
+      <c r="O28" s="1">
+        <v>17302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1">
+        <v>198856.5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>57514.1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>59829</v>
+      </c>
+      <c r="G29">
+        <v>64</v>
+      </c>
+      <c r="H29" s="1">
+        <v>200329.1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>56290.5</v>
+      </c>
+      <c r="J29" s="1">
+        <v>58186</v>
+      </c>
+      <c r="L29">
+        <v>64</v>
+      </c>
+      <c r="M29" s="1">
+        <v>255877.8</v>
+      </c>
+      <c r="N29" s="1">
+        <v>67790.2</v>
+      </c>
+      <c r="O29" s="1">
+        <v>69409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>256</v>
+      </c>
+      <c r="C30" s="1">
+        <v>793702.8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>229915.2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>236437</v>
+      </c>
+      <c r="G30">
+        <v>256</v>
+      </c>
+      <c r="H30" s="1">
+        <v>799601</v>
+      </c>
+      <c r="I30" s="1">
+        <v>224946.6</v>
+      </c>
+      <c r="J30" s="1">
+        <v>231035</v>
+      </c>
+      <c r="L30">
+        <v>256</v>
+      </c>
+      <c r="M30" s="1">
+        <v>999672</v>
+      </c>
+      <c r="N30" s="1">
+        <v>271312.3</v>
+      </c>
+      <c r="O30" s="1">
+        <v>275993</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>400</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+      <c r="L48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>2</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N49" t="s">
+        <v>1</v>
+      </c>
+      <c r="O49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3772.3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1567.8</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1680</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+      <c r="H50" s="1">
+        <v>3849.7</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1570.7</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1669.5</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="M50" s="1">
+        <v>5009.7</v>
+      </c>
+      <c r="N50" s="1">
+        <v>2013.1</v>
+      </c>
+      <c r="O50" s="1">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>16</v>
+      </c>
+      <c r="C51" s="1">
+        <v>15083.6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>8175.8</v>
+      </c>
+      <c r="E51" s="1">
+        <v>8607.7000000000007</v>
+      </c>
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51" s="1">
+        <v>15581.9</v>
+      </c>
+      <c r="I51" s="1">
+        <v>7754.2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>8350.6</v>
+      </c>
+      <c r="L51">
+        <v>16</v>
+      </c>
+      <c r="M51" s="1">
+        <v>20233.5</v>
+      </c>
+      <c r="N51" s="1">
+        <v>9010.4</v>
+      </c>
+      <c r="O51" s="1">
+        <v>9786.9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>64</v>
+      </c>
+      <c r="C52" s="1">
+        <v>60250.9</v>
+      </c>
+      <c r="D52" s="1">
+        <v>32501.5</v>
+      </c>
+      <c r="E52" s="1">
+        <v>34919.699999999997</v>
+      </c>
+      <c r="G52">
+        <v>64</v>
+      </c>
+      <c r="H52" s="1">
+        <v>61686.3</v>
+      </c>
+      <c r="I52" s="1">
+        <v>29593.5</v>
+      </c>
+      <c r="J52" s="1">
+        <v>32279.7</v>
+      </c>
+      <c r="L52">
+        <v>64</v>
+      </c>
+      <c r="M52" s="1">
+        <v>80070.399999999994</v>
+      </c>
+      <c r="N52" s="1">
+        <v>35544.199999999997</v>
+      </c>
+      <c r="O52" s="1">
+        <v>37831.800000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>256</v>
+      </c>
+      <c r="C53" s="1">
+        <v>242848.6</v>
+      </c>
+      <c r="D53" s="1">
+        <v>125720.2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>135913</v>
+      </c>
+      <c r="G53">
+        <v>256</v>
+      </c>
+      <c r="H53" s="1">
+        <v>255410.6</v>
+      </c>
+      <c r="I53" s="1">
+        <v>118001.5</v>
+      </c>
+      <c r="J53" s="1">
+        <v>126670.5</v>
+      </c>
+      <c r="L53">
+        <v>256</v>
+      </c>
+      <c r="M53" s="1">
+        <v>328751.8</v>
+      </c>
+      <c r="N53" s="1">
+        <v>139375.4</v>
+      </c>
+      <c r="O53" s="1">
+        <v>150865.20000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>400</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" t="s">
+        <v>5</v>
+      </c>
+      <c r="M69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>2</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J70" t="s">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>0</v>
+      </c>
+      <c r="M70" t="s">
+        <v>2</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O70" t="s">
+        <v>1</v>
+      </c>
+      <c r="P70" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="H71">
+        <v>4</v>
+      </c>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="M71">
+        <v>4</v>
+      </c>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>16</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="H72">
+        <v>16</v>
+      </c>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="M72">
+        <v>16</v>
+      </c>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>64</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="H73">
+        <v>64</v>
+      </c>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="M73">
+        <v>64</v>
+      </c>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>256</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="H74">
+        <v>256</v>
+      </c>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="M74">
+        <v>256</v>
+      </c>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gonna have to do the report on the macbook, PC's fucked
</commit_message>
<xml_diff>
--- a/CW1/Graphs/Graphs.xlsx
+++ b/CW1/Graphs/Graphs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW1\Graphs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
@@ -17,12 +12,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -59,8 +49,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +58,317 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -85,18 +376,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -104,17 +587,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -160,7 +640,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -224,7 +703,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2AEC-4497-AAE8-84B929552E10}"/>
             </c:ext>
@@ -285,7 +764,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2AEC-4497-AAE8-84B929552E10}"/>
             </c:ext>
@@ -322,7 +801,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2AEC-4497-AAE8-84B929552E10}"/>
             </c:ext>
@@ -336,12 +815,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="140306304"/>
+        <c:axId val="65216512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="140306304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,14 +848,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65216512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -383,7 +862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65216512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,21 +885,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="140306304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -436,9 +913,9 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -548,7 +1025,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B703-4282-A711-884D22CA7167}"/>
             </c:ext>
@@ -609,7 +1086,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B703-4282-A711-884D22CA7167}"/>
             </c:ext>
@@ -646,7 +1123,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B703-4282-A711-884D22CA7167}"/>
             </c:ext>
@@ -660,12 +1137,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65532288"/>
+        <c:axId val="65534208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65532288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +1177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65534208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -707,7 +1185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65534208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +1215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65532288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -760,9 +1238,9 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -856,11 +1334,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26567.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105660.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>426819.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1652563</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACAC-404C-9D7A-C7B288F8DF0E}"/>
             </c:ext>
@@ -905,11 +1395,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13498.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50764.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>204060.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>805825</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACAC-404C-9D7A-C7B288F8DF0E}"/>
             </c:ext>
@@ -930,11 +1432,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13601.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53075.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>219116.79999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>892637.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ACAC-404C-9D7A-C7B288F8DF0E}"/>
             </c:ext>
@@ -948,12 +1462,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65586688"/>
+        <c:axId val="65588608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65586688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -987,7 +1502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65588608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -995,7 +1510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65588608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65586688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1048,9 +1563,9 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1144,11 +1659,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>38280.699999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136265.79999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>564249.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2159342</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D988-4D63-BDDA-B06AF0D44524}"/>
             </c:ext>
@@ -1193,11 +1720,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15527.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>239772.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>952495</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D988-4D63-BDDA-B06AF0D44524}"/>
             </c:ext>
@@ -1218,11 +1757,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15916</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62556.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>258207.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1022660.7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D988-4D63-BDDA-B06AF0D44524}"/>
             </c:ext>
@@ -1236,12 +1787,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="66136704"/>
+        <c:axId val="66159360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="66136704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,7 +1827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="66159360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1283,7 +1835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="66159360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="66136704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,9 +1888,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1384,7 +1936,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1448,7 +1999,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D5B-4804-8CDC-FD1533CEB3B2}"/>
             </c:ext>
@@ -1509,7 +2060,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8D5B-4804-8CDC-FD1533CEB3B2}"/>
             </c:ext>
@@ -1546,7 +2097,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8D5B-4804-8CDC-FD1533CEB3B2}"/>
             </c:ext>
@@ -1560,12 +2111,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65256448"/>
+        <c:axId val="65258624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65256448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,14 +2144,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65258624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1607,7 +2158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65258624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,21 +2181,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65256448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1660,9 +2209,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1708,7 +2257,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1772,7 +2320,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3FD7-4005-9B94-586CB283C417}"/>
             </c:ext>
@@ -1833,7 +2381,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3FD7-4005-9B94-586CB283C417}"/>
             </c:ext>
@@ -1870,7 +2418,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3FD7-4005-9B94-586CB283C417}"/>
             </c:ext>
@@ -1884,12 +2432,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65163648"/>
+        <c:axId val="65165568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65163648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,14 +2465,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65165568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1931,7 +2479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65165568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,21 +2502,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65163648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1984,9 +2530,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2096,7 +2642,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6CD5-4635-96AA-EA77268F7153}"/>
             </c:ext>
@@ -2157,7 +2703,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6CD5-4635-96AA-EA77268F7153}"/>
             </c:ext>
@@ -2194,7 +2740,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6CD5-4635-96AA-EA77268F7153}"/>
             </c:ext>
@@ -2208,12 +2754,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65283584"/>
+        <c:axId val="65285504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65283584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +2794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65285504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2255,7 +2802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65285504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,7 +2832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65283584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2308,9 +2855,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2420,7 +2967,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2A5C-40E0-AA96-233F7ED22E7B}"/>
             </c:ext>
@@ -2481,7 +3028,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2A5C-40E0-AA96-233F7ED22E7B}"/>
             </c:ext>
@@ -2518,7 +3065,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2A5C-40E0-AA96-233F7ED22E7B}"/>
             </c:ext>
@@ -2532,12 +3079,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65319296"/>
+        <c:axId val="65321216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65319296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +3119,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65321216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2579,7 +3127,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65321216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,7 +3157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65319296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2632,9 +3180,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2744,7 +3292,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F311-4D89-91E6-34226ACF039C}"/>
             </c:ext>
@@ -2805,7 +3353,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F311-4D89-91E6-34226ACF039C}"/>
             </c:ext>
@@ -2842,7 +3390,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F311-4D89-91E6-34226ACF039C}"/>
             </c:ext>
@@ -2856,12 +3404,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65429888"/>
+        <c:axId val="65431808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65429888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2895,7 +3444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65431808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2903,7 +3452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65431808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,7 +3482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65429888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2956,9 +3505,9 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3068,7 +3617,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4411-4C68-A7C2-2A64EA2AE011}"/>
             </c:ext>
@@ -3129,7 +3678,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4411-4C68-A7C2-2A64EA2AE011}"/>
             </c:ext>
@@ -3166,7 +3715,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-4411-4C68-A7C2-2A64EA2AE011}"/>
             </c:ext>
@@ -3180,12 +3729,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65463808"/>
+        <c:axId val="65465728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65463808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,7 +3769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65465728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3227,7 +3777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65465728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3257,7 +3807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65463808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3280,9 +3830,9 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3376,11 +3926,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25766.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108437.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>415926.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1683655.8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-230E-421D-9EA8-2B8A295308D9}"/>
             </c:ext>
@@ -3425,11 +3987,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12029.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55705.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>217248.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>874755.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-230E-421D-9EA8-2B8A295308D9}"/>
             </c:ext>
@@ -3450,11 +4024,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12642.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56926.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>229301.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>955163.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-230E-421D-9EA8-2B8A295308D9}"/>
             </c:ext>
@@ -3468,12 +4054,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65775872"/>
+        <c:axId val="65778048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65775872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3507,7 +4094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65778048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3515,7 +4102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65778048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3545,7 +4132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65775872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3568,9 +4155,9 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3680,7 +4267,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6042-4FA0-9A12-58EE72AD66AD}"/>
             </c:ext>
@@ -3741,7 +4328,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6042-4FA0-9A12-58EE72AD66AD}"/>
             </c:ext>
@@ -3778,7 +4365,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6042-4FA0-9A12-58EE72AD66AD}"/>
             </c:ext>
@@ -3792,12 +4379,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39597184"/>
-        <c:axId val="39599488"/>
+        <c:axId val="65498112"/>
+        <c:axId val="65500288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39597184"/>
+        <c:axId val="65498112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3831,7 +4419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599488"/>
+        <c:crossAx val="65500288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3839,7 +4427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39599488"/>
+        <c:axId val="65500288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3869,7 +4457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39597184"/>
+        <c:crossAx val="65498112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4362,7 +4950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4397,7 +4985,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4574,7 +5162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4584,8 +5172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,81 +6003,153 @@
       <c r="C71">
         <v>4</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="D71" s="1">
+        <v>25766.5</v>
+      </c>
+      <c r="E71" s="1">
+        <v>12029.3</v>
+      </c>
+      <c r="F71" s="1">
+        <v>12642.7</v>
+      </c>
       <c r="H71">
         <v>4</v>
       </c>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
+      <c r="I71" s="1">
+        <v>26567.9</v>
+      </c>
+      <c r="J71" s="1">
+        <v>13498.3</v>
+      </c>
+      <c r="K71" s="1">
+        <v>13601.5</v>
+      </c>
       <c r="M71">
         <v>4</v>
       </c>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
+      <c r="N71" s="1">
+        <v>38280.699999999997</v>
+      </c>
+      <c r="O71" s="1">
+        <v>15527.5</v>
+      </c>
+      <c r="P71" s="1">
+        <v>15916</v>
+      </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>16</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="D72" s="1">
+        <v>108437.6</v>
+      </c>
+      <c r="E72" s="1">
+        <v>55705.5</v>
+      </c>
+      <c r="F72" s="1">
+        <v>56926.6</v>
+      </c>
       <c r="H72">
         <v>16</v>
       </c>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
+      <c r="I72" s="1">
+        <v>105660.5</v>
+      </c>
+      <c r="J72" s="1">
+        <v>50764.1</v>
+      </c>
+      <c r="K72" s="1">
+        <v>53075.7</v>
+      </c>
       <c r="M72">
         <v>16</v>
       </c>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
+      <c r="N72" s="1">
+        <v>136265.79999999999</v>
+      </c>
+      <c r="O72" s="1">
+        <v>58945</v>
+      </c>
+      <c r="P72" s="1">
+        <v>62556.1</v>
+      </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>64</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="D73" s="1">
+        <v>415926.2</v>
+      </c>
+      <c r="E73" s="1">
+        <v>217248.6</v>
+      </c>
+      <c r="F73" s="1">
+        <v>229301.7</v>
+      </c>
       <c r="H73">
         <v>64</v>
       </c>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
+      <c r="I73" s="1">
+        <v>426819.2</v>
+      </c>
+      <c r="J73" s="1">
+        <v>204060.4</v>
+      </c>
+      <c r="K73" s="1">
+        <v>219116.79999999999</v>
+      </c>
       <c r="M73">
         <v>64</v>
       </c>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
+      <c r="N73" s="1">
+        <v>564249.9</v>
+      </c>
+      <c r="O73" s="1">
+        <v>239772.3</v>
+      </c>
+      <c r="P73" s="1">
+        <v>258207.5</v>
+      </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>256</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="D74" s="1">
+        <v>1683655.8</v>
+      </c>
+      <c r="E74" s="1">
+        <v>874755.75</v>
+      </c>
+      <c r="F74" s="1">
+        <v>955163.4</v>
+      </c>
       <c r="H74">
         <v>256</v>
       </c>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
+      <c r="I74" s="1">
+        <v>1652563</v>
+      </c>
+      <c r="J74" s="2">
+        <v>805825</v>
+      </c>
+      <c r="K74" s="1">
+        <v>892637.3</v>
+      </c>
       <c r="M74">
         <v>256</v>
       </c>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
+      <c r="N74" s="1">
+        <v>2159342</v>
+      </c>
+      <c r="O74" s="1">
+        <v>952495</v>
+      </c>
+      <c r="P74" s="1">
+        <v>1022660.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>